<commit_message>
Find new optimal diet
</commit_message>
<xml_diff>
--- a/Data/nut_constraints.xlsx
+++ b/Data/nut_constraints.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f96c677c7dacd35b/Documents/Derek's stuff/Not School/Ongoing Personal Interests and Files/Computer Science/Nutrition-Optimization/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\derek\OneDrive\Documents\Derek's stuff\Not School\Ongoing Personal Interests and Files\Computer Science\Nutrition-Optimization-New\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{B98729F0-8560-40CB-9A89-B0E18BAB0735}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{0463E1FA-F0A4-44AB-959A-E8CCA3F0061B}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{B98729F0-8560-40CB-9A89-B0E18BAB0735}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{C09DD064-1E72-4BC2-A119-36725AF1049F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{020B6AF4-CACA-4C87-9277-984FC57AE6C4}"/>
   </bookViews>
@@ -831,7 +831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F24CE3E-4917-484F-A901-989C2E03DB27}">
   <dimension ref="B1:ET4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CJ1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:ET4"/>
     </sheetView>
   </sheetViews>
@@ -1782,7 +1782,7 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="S3" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
add images for readme
</commit_message>
<xml_diff>
--- a/Data/nut_constraints.xlsx
+++ b/Data/nut_constraints.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\derek\OneDrive\Documents\Derek's stuff\Not School\Ongoing Personal Interests and Files\Computer Science\Nutrition-Optimization-New\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f96c677c7dacd35b/Documents/Derek's stuff/Not School/Ongoing Personal Interests and Files/Computer Science/Nutrition-Optimization-New/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{B98729F0-8560-40CB-9A89-B0E18BAB0735}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{C09DD064-1E72-4BC2-A119-36725AF1049F}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="102_{71955CBC-F00A-4639-A298-521CB3F5D045}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{AFC89AE6-2DB0-41BF-AC42-692494CBCC57}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{020B6AF4-CACA-4C87-9277-984FC57AE6C4}"/>
   </bookViews>
@@ -31,453 +31,453 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="149">
+  <si>
+    <t>['Protein',</t>
+  </si>
+  <si>
+    <t>Total lipid (fat),</t>
+  </si>
+  <si>
+    <t>Carbohydrate, by difference,</t>
+  </si>
+  <si>
+    <t>Ash,</t>
+  </si>
+  <si>
+    <t>Energy,</t>
+  </si>
+  <si>
+    <t>Starch,</t>
+  </si>
+  <si>
+    <t>Sucrose,</t>
+  </si>
+  <si>
+    <t>Glucose (dextrose),</t>
+  </si>
+  <si>
+    <t>Fructose,</t>
+  </si>
+  <si>
+    <t>Lactose,</t>
+  </si>
+  <si>
+    <t>Maltose,</t>
+  </si>
+  <si>
+    <t>Alcohol, ethyl,</t>
+  </si>
+  <si>
+    <t>Water,</t>
+  </si>
+  <si>
+    <t>Caffeine,</t>
+  </si>
+  <si>
+    <t>Theobromine,</t>
+  </si>
+  <si>
+    <t>Sugars, total,</t>
+  </si>
+  <si>
+    <t>Galactose,</t>
+  </si>
+  <si>
+    <t>Fiber, total dietary,</t>
+  </si>
+  <si>
+    <t>Calcium, Ca,</t>
+  </si>
+  <si>
+    <t>Iron, Fe,</t>
+  </si>
+  <si>
+    <t>Magnesium, Mg,</t>
+  </si>
+  <si>
+    <t>Phosphorus, P,</t>
+  </si>
+  <si>
+    <t>Potassium, K,</t>
+  </si>
+  <si>
+    <t>Sodium, Na,</t>
+  </si>
+  <si>
+    <t>Zinc, Zn,</t>
+  </si>
+  <si>
+    <t>Copper, Cu,</t>
+  </si>
+  <si>
+    <t>Fluoride, F,</t>
+  </si>
+  <si>
+    <t>Manganese, Mn,</t>
+  </si>
+  <si>
+    <t>Selenium, Se,</t>
+  </si>
+  <si>
+    <t>Vitamin A, IU,</t>
+  </si>
+  <si>
+    <t>Retinol,</t>
+  </si>
+  <si>
+    <t>Vitamin A, RAE,</t>
+  </si>
+  <si>
+    <t>Carotene, beta,</t>
+  </si>
+  <si>
+    <t>Carotene, alpha,</t>
+  </si>
+  <si>
+    <t>Vitamin E (alpha-tocopherol),</t>
+  </si>
+  <si>
+    <t>Vitamin D,</t>
+  </si>
+  <si>
+    <t>Vitamin D2 (ergocalciferol),</t>
+  </si>
+  <si>
+    <t>Vitamin D3 (cholecalciferol),</t>
+  </si>
+  <si>
+    <t>Vitamin D (D2 + D3),</t>
+  </si>
+  <si>
+    <t>Cryptoxanthin, beta,</t>
+  </si>
+  <si>
+    <t>Lycopene,</t>
+  </si>
+  <si>
+    <t>Lutein + zeaxanthin,</t>
+  </si>
+  <si>
+    <t>Tocopherol, beta,</t>
+  </si>
+  <si>
+    <t>Tocopherol, gamma,</t>
+  </si>
+  <si>
+    <t>Tocopherol, delta,</t>
+  </si>
+  <si>
+    <t>Tocotrienol, alpha,</t>
+  </si>
+  <si>
+    <t>Tocotrienol, beta,</t>
+  </si>
+  <si>
+    <t>Tocotrienol, gamma,</t>
+  </si>
+  <si>
+    <t>Tocotrienol, delta,</t>
+  </si>
+  <si>
+    <t>Vitamin C, total ascorbic acid,</t>
+  </si>
+  <si>
+    <t>Thiamin,</t>
+  </si>
+  <si>
+    <t>Riboflavin,</t>
+  </si>
+  <si>
+    <t>Niacin,</t>
+  </si>
+  <si>
+    <t>Pantothenic acid,</t>
+  </si>
+  <si>
+    <t>Vitamin B-6,</t>
+  </si>
+  <si>
+    <t>Folate, total,</t>
+  </si>
+  <si>
+    <t>Vitamin B-12,</t>
+  </si>
+  <si>
+    <t>Choline, total,</t>
+  </si>
+  <si>
+    <t>Menaquinone-4,</t>
+  </si>
+  <si>
+    <t>Dihydrophylloquinone,</t>
+  </si>
+  <si>
+    <t>Vitamin K (phylloquinone),</t>
+  </si>
+  <si>
+    <t>Folic acid,</t>
+  </si>
+  <si>
+    <t>Folate, food,</t>
+  </si>
+  <si>
+    <t>Folate, DFE,</t>
+  </si>
+  <si>
+    <t>Betaine,</t>
+  </si>
+  <si>
+    <t>Tryptophan,</t>
+  </si>
+  <si>
+    <t>Threonine,</t>
+  </si>
+  <si>
+    <t>Isoleucine,</t>
+  </si>
+  <si>
+    <t>Leucine,</t>
+  </si>
+  <si>
+    <t>Lysine,</t>
+  </si>
+  <si>
+    <t>Methionine,</t>
+  </si>
+  <si>
+    <t>Cystine,</t>
+  </si>
+  <si>
+    <t>Phenylalanine,</t>
+  </si>
+  <si>
+    <t>Tyrosine,</t>
+  </si>
+  <si>
+    <t>Valine,</t>
+  </si>
+  <si>
+    <t>Arginine,</t>
+  </si>
+  <si>
+    <t>Histidine,</t>
+  </si>
+  <si>
+    <t>Alanine,</t>
+  </si>
+  <si>
+    <t>Aspartic acid,</t>
+  </si>
+  <si>
+    <t>Glutamic acid,</t>
+  </si>
+  <si>
+    <t>Glycine,</t>
+  </si>
+  <si>
+    <t>Proline,</t>
+  </si>
+  <si>
+    <t>Serine,</t>
+  </si>
+  <si>
+    <t>Hydroxyproline,</t>
+  </si>
+  <si>
+    <t>Vitamin E, added,</t>
+  </si>
+  <si>
+    <t>Vitamin B-12, added,</t>
+  </si>
+  <si>
+    <t>Fatty acids, total trans,</t>
+  </si>
+  <si>
+    <t>Fatty acids, total saturated,</t>
+  </si>
+  <si>
+    <t>4:0,</t>
+  </si>
+  <si>
+    <t>6:0,</t>
+  </si>
+  <si>
+    <t>8:0,</t>
+  </si>
+  <si>
+    <t>10:0,</t>
+  </si>
+  <si>
+    <t>12:0,</t>
+  </si>
+  <si>
+    <t>14:0,</t>
+  </si>
+  <si>
+    <t>16:0,</t>
+  </si>
+  <si>
+    <t>18:0,</t>
+  </si>
+  <si>
+    <t>20:0,</t>
+  </si>
+  <si>
+    <t>18:1 undifferentiated,</t>
+  </si>
+  <si>
+    <t>18:2 undifferentiated,</t>
+  </si>
+  <si>
+    <t>18:3 undifferentiated,</t>
+  </si>
+  <si>
+    <t>20:4 undifferentiated,</t>
+  </si>
+  <si>
+    <t>22:6 n-3 (DHA),</t>
+  </si>
+  <si>
+    <t>22:0,</t>
+  </si>
+  <si>
+    <t>14:1,</t>
+  </si>
+  <si>
+    <t>16:1 undifferentiated,</t>
+  </si>
+  <si>
+    <t>18:4,</t>
+  </si>
+  <si>
+    <t>20:1,</t>
+  </si>
+  <si>
+    <t>20:5 n-3 (EPA),</t>
+  </si>
+  <si>
+    <t>22:1 undifferentiated,</t>
+  </si>
+  <si>
+    <t>22:5 n-3 (DPA),</t>
+  </si>
+  <si>
+    <t>Phytosterols,</t>
+  </si>
+  <si>
+    <t>Stigmasterol,</t>
+  </si>
+  <si>
+    <t>Campesterol,</t>
+  </si>
+  <si>
+    <t>Beta-sitosterol,</t>
+  </si>
+  <si>
+    <t>Fatty acids, total monounsaturated,</t>
+  </si>
+  <si>
+    <t>Fatty acids, total polyunsaturated,</t>
+  </si>
+  <si>
+    <t>15:0,</t>
+  </si>
+  <si>
+    <t>17:0,</t>
+  </si>
+  <si>
+    <t>24:0,</t>
+  </si>
+  <si>
+    <t>16:1 t,</t>
+  </si>
+  <si>
+    <t>18:1 t,</t>
+  </si>
+  <si>
+    <t>22:1 t,</t>
+  </si>
+  <si>
+    <t>18:2 t not further defined,</t>
+  </si>
+  <si>
+    <t>18:2 i,</t>
+  </si>
+  <si>
+    <t>18:2 t,t,</t>
+  </si>
+  <si>
+    <t>18:2 CLAs,</t>
+  </si>
+  <si>
+    <t>24:1 c,</t>
+  </si>
+  <si>
+    <t>20:2 n-6 c,c,</t>
+  </si>
+  <si>
+    <t>16:1 c,</t>
+  </si>
+  <si>
+    <t>18:1 c,</t>
+  </si>
+  <si>
+    <t>18:2 n-6 c,c,</t>
+  </si>
+  <si>
+    <t>22:1 c,</t>
+  </si>
+  <si>
+    <t>18:3 n-6 c,c,c,</t>
+  </si>
+  <si>
+    <t>17:1,</t>
+  </si>
+  <si>
+    <t>20:3 undifferentiated,</t>
+  </si>
+  <si>
+    <t>Fatty acids, total trans-monoenoic,</t>
+  </si>
+  <si>
+    <t>Fatty acids, total trans-polyenoic,</t>
+  </si>
+  <si>
+    <t>13:0,</t>
+  </si>
+  <si>
+    <t>15:1,</t>
+  </si>
+  <si>
+    <t>18:3 n-3 c,c,c (ALA),</t>
+  </si>
+  <si>
+    <t>20:3 n-3,</t>
+  </si>
+  <si>
+    <t>20:3 n-6,</t>
+  </si>
+  <si>
+    <t>20:4 n-6,</t>
+  </si>
+  <si>
+    <t>18:3i,</t>
+  </si>
+  <si>
+    <t>21:5,</t>
+  </si>
+  <si>
+    <t>22:4,</t>
+  </si>
+  <si>
+    <t>18:1-11 t (18:1t n-7)]</t>
+  </si>
+  <si>
+    <t>Cholesterol, (note changed to force eggs 2/10/19 from 200 mg)</t>
+  </si>
   <si>
     <t/>
-  </si>
-  <si>
-    <t>['Protein',</t>
-  </si>
-  <si>
-    <t>Total lipid (fat),</t>
-  </si>
-  <si>
-    <t>Carbohydrate, by difference,</t>
-  </si>
-  <si>
-    <t>Ash,</t>
-  </si>
-  <si>
-    <t>Energy,</t>
-  </si>
-  <si>
-    <t>Starch,</t>
-  </si>
-  <si>
-    <t>Sucrose,</t>
-  </si>
-  <si>
-    <t>Glucose (dextrose),</t>
-  </si>
-  <si>
-    <t>Fructose,</t>
-  </si>
-  <si>
-    <t>Lactose,</t>
-  </si>
-  <si>
-    <t>Maltose,</t>
-  </si>
-  <si>
-    <t>Alcohol, ethyl,</t>
-  </si>
-  <si>
-    <t>Water,</t>
-  </si>
-  <si>
-    <t>Caffeine,</t>
-  </si>
-  <si>
-    <t>Theobromine,</t>
-  </si>
-  <si>
-    <t>Sugars, total,</t>
-  </si>
-  <si>
-    <t>Galactose,</t>
-  </si>
-  <si>
-    <t>Fiber, total dietary,</t>
-  </si>
-  <si>
-    <t>Calcium, Ca,</t>
-  </si>
-  <si>
-    <t>Iron, Fe,</t>
-  </si>
-  <si>
-    <t>Magnesium, Mg,</t>
-  </si>
-  <si>
-    <t>Phosphorus, P,</t>
-  </si>
-  <si>
-    <t>Potassium, K,</t>
-  </si>
-  <si>
-    <t>Sodium, Na,</t>
-  </si>
-  <si>
-    <t>Zinc, Zn,</t>
-  </si>
-  <si>
-    <t>Copper, Cu,</t>
-  </si>
-  <si>
-    <t>Fluoride, F,</t>
-  </si>
-  <si>
-    <t>Manganese, Mn,</t>
-  </si>
-  <si>
-    <t>Selenium, Se,</t>
-  </si>
-  <si>
-    <t>Vitamin A, IU,</t>
-  </si>
-  <si>
-    <t>Retinol,</t>
-  </si>
-  <si>
-    <t>Vitamin A, RAE,</t>
-  </si>
-  <si>
-    <t>Carotene, beta,</t>
-  </si>
-  <si>
-    <t>Carotene, alpha,</t>
-  </si>
-  <si>
-    <t>Vitamin E (alpha-tocopherol),</t>
-  </si>
-  <si>
-    <t>Vitamin D,</t>
-  </si>
-  <si>
-    <t>Vitamin D2 (ergocalciferol),</t>
-  </si>
-  <si>
-    <t>Vitamin D3 (cholecalciferol),</t>
-  </si>
-  <si>
-    <t>Vitamin D (D2 + D3),</t>
-  </si>
-  <si>
-    <t>Cryptoxanthin, beta,</t>
-  </si>
-  <si>
-    <t>Lycopene,</t>
-  </si>
-  <si>
-    <t>Lutein + zeaxanthin,</t>
-  </si>
-  <si>
-    <t>Tocopherol, beta,</t>
-  </si>
-  <si>
-    <t>Tocopherol, gamma,</t>
-  </si>
-  <si>
-    <t>Tocopherol, delta,</t>
-  </si>
-  <si>
-    <t>Tocotrienol, alpha,</t>
-  </si>
-  <si>
-    <t>Tocotrienol, beta,</t>
-  </si>
-  <si>
-    <t>Tocotrienol, gamma,</t>
-  </si>
-  <si>
-    <t>Tocotrienol, delta,</t>
-  </si>
-  <si>
-    <t>Vitamin C, total ascorbic acid,</t>
-  </si>
-  <si>
-    <t>Thiamin,</t>
-  </si>
-  <si>
-    <t>Riboflavin,</t>
-  </si>
-  <si>
-    <t>Niacin,</t>
-  </si>
-  <si>
-    <t>Pantothenic acid,</t>
-  </si>
-  <si>
-    <t>Vitamin B-6,</t>
-  </si>
-  <si>
-    <t>Folate, total,</t>
-  </si>
-  <si>
-    <t>Vitamin B-12,</t>
-  </si>
-  <si>
-    <t>Choline, total,</t>
-  </si>
-  <si>
-    <t>Menaquinone-4,</t>
-  </si>
-  <si>
-    <t>Dihydrophylloquinone,</t>
-  </si>
-  <si>
-    <t>Vitamin K (phylloquinone),</t>
-  </si>
-  <si>
-    <t>Folic acid,</t>
-  </si>
-  <si>
-    <t>Folate, food,</t>
-  </si>
-  <si>
-    <t>Folate, DFE,</t>
-  </si>
-  <si>
-    <t>Betaine,</t>
-  </si>
-  <si>
-    <t>Tryptophan,</t>
-  </si>
-  <si>
-    <t>Threonine,</t>
-  </si>
-  <si>
-    <t>Isoleucine,</t>
-  </si>
-  <si>
-    <t>Leucine,</t>
-  </si>
-  <si>
-    <t>Lysine,</t>
-  </si>
-  <si>
-    <t>Methionine,</t>
-  </si>
-  <si>
-    <t>Cystine,</t>
-  </si>
-  <si>
-    <t>Phenylalanine,</t>
-  </si>
-  <si>
-    <t>Tyrosine,</t>
-  </si>
-  <si>
-    <t>Valine,</t>
-  </si>
-  <si>
-    <t>Arginine,</t>
-  </si>
-  <si>
-    <t>Histidine,</t>
-  </si>
-  <si>
-    <t>Alanine,</t>
-  </si>
-  <si>
-    <t>Aspartic acid,</t>
-  </si>
-  <si>
-    <t>Glutamic acid,</t>
-  </si>
-  <si>
-    <t>Glycine,</t>
-  </si>
-  <si>
-    <t>Proline,</t>
-  </si>
-  <si>
-    <t>Serine,</t>
-  </si>
-  <si>
-    <t>Hydroxyproline,</t>
-  </si>
-  <si>
-    <t>Vitamin E, added,</t>
-  </si>
-  <si>
-    <t>Vitamin B-12, added,</t>
-  </si>
-  <si>
-    <t>Fatty acids, total trans,</t>
-  </si>
-  <si>
-    <t>Fatty acids, total saturated,</t>
-  </si>
-  <si>
-    <t>4:0,</t>
-  </si>
-  <si>
-    <t>6:0,</t>
-  </si>
-  <si>
-    <t>8:0,</t>
-  </si>
-  <si>
-    <t>10:0,</t>
-  </si>
-  <si>
-    <t>12:0,</t>
-  </si>
-  <si>
-    <t>14:0,</t>
-  </si>
-  <si>
-    <t>16:0,</t>
-  </si>
-  <si>
-    <t>18:0,</t>
-  </si>
-  <si>
-    <t>20:0,</t>
-  </si>
-  <si>
-    <t>18:1 undifferentiated,</t>
-  </si>
-  <si>
-    <t>18:2 undifferentiated,</t>
-  </si>
-  <si>
-    <t>18:3 undifferentiated,</t>
-  </si>
-  <si>
-    <t>20:4 undifferentiated,</t>
-  </si>
-  <si>
-    <t>22:6 n-3 (DHA),</t>
-  </si>
-  <si>
-    <t>22:0,</t>
-  </si>
-  <si>
-    <t>14:1,</t>
-  </si>
-  <si>
-    <t>16:1 undifferentiated,</t>
-  </si>
-  <si>
-    <t>18:4,</t>
-  </si>
-  <si>
-    <t>20:1,</t>
-  </si>
-  <si>
-    <t>20:5 n-3 (EPA),</t>
-  </si>
-  <si>
-    <t>22:1 undifferentiated,</t>
-  </si>
-  <si>
-    <t>22:5 n-3 (DPA),</t>
-  </si>
-  <si>
-    <t>Phytosterols,</t>
-  </si>
-  <si>
-    <t>Stigmasterol,</t>
-  </si>
-  <si>
-    <t>Campesterol,</t>
-  </si>
-  <si>
-    <t>Beta-sitosterol,</t>
-  </si>
-  <si>
-    <t>Fatty acids, total monounsaturated,</t>
-  </si>
-  <si>
-    <t>Fatty acids, total polyunsaturated,</t>
-  </si>
-  <si>
-    <t>15:0,</t>
-  </si>
-  <si>
-    <t>17:0,</t>
-  </si>
-  <si>
-    <t>24:0,</t>
-  </si>
-  <si>
-    <t>16:1 t,</t>
-  </si>
-  <si>
-    <t>18:1 t,</t>
-  </si>
-  <si>
-    <t>22:1 t,</t>
-  </si>
-  <si>
-    <t>18:2 t not further defined,</t>
-  </si>
-  <si>
-    <t>18:2 i,</t>
-  </si>
-  <si>
-    <t>18:2 t,t,</t>
-  </si>
-  <si>
-    <t>18:2 CLAs,</t>
-  </si>
-  <si>
-    <t>24:1 c,</t>
-  </si>
-  <si>
-    <t>20:2 n-6 c,c,</t>
-  </si>
-  <si>
-    <t>16:1 c,</t>
-  </si>
-  <si>
-    <t>18:1 c,</t>
-  </si>
-  <si>
-    <t>18:2 n-6 c,c,</t>
-  </si>
-  <si>
-    <t>22:1 c,</t>
-  </si>
-  <si>
-    <t>18:3 n-6 c,c,c,</t>
-  </si>
-  <si>
-    <t>17:1,</t>
-  </si>
-  <si>
-    <t>20:3 undifferentiated,</t>
-  </si>
-  <si>
-    <t>Fatty acids, total trans-monoenoic,</t>
-  </si>
-  <si>
-    <t>Fatty acids, total trans-polyenoic,</t>
-  </si>
-  <si>
-    <t>13:0,</t>
-  </si>
-  <si>
-    <t>15:1,</t>
-  </si>
-  <si>
-    <t>18:3 n-3 c,c,c (ALA),</t>
-  </si>
-  <si>
-    <t>20:3 n-3,</t>
-  </si>
-  <si>
-    <t>20:3 n-6,</t>
-  </si>
-  <si>
-    <t>20:4 n-6,</t>
-  </si>
-  <si>
-    <t>18:3i,</t>
-  </si>
-  <si>
-    <t>21:5,</t>
-  </si>
-  <si>
-    <t>22:4,</t>
-  </si>
-  <si>
-    <t>18:1-11 t (18:1t n-7)]</t>
-  </si>
-  <si>
-    <t>Cholesterol, (note changed to force eggs 2/10/19 from 200 mg)</t>
   </si>
 </sst>
 </file>
@@ -493,12 +493,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -513,8 +525,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -839,451 +853,451 @@
   <sheetData>
     <row r="1" spans="2:150" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
-        <v>5</v>
-      </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>36</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>38</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>39</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>40</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>41</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>42</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>43</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>44</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>45</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>46</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>47</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>48</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>49</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>50</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>51</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>52</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>53</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>54</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>55</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>56</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>57</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>58</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>59</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>60</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>61</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>62</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>63</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BO1" t="s">
         <v>64</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BP1" t="s">
         <v>65</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BQ1" t="s">
         <v>66</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BR1" t="s">
         <v>67</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BS1" t="s">
         <v>68</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BT1" t="s">
         <v>69</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BU1" t="s">
         <v>70</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BV1" t="s">
         <v>71</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="BW1" t="s">
         <v>72</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="BX1" t="s">
         <v>73</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="BY1" t="s">
         <v>74</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="BZ1" t="s">
         <v>75</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CA1" t="s">
         <v>76</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CB1" t="s">
         <v>77</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CC1" t="s">
         <v>78</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CD1" t="s">
         <v>79</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CE1" t="s">
         <v>80</v>
       </c>
-      <c r="CE1" t="s">
+      <c r="CF1" t="s">
         <v>81</v>
       </c>
-      <c r="CF1" t="s">
+      <c r="CG1" t="s">
         <v>82</v>
       </c>
-      <c r="CG1" t="s">
+      <c r="CH1" t="s">
         <v>83</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="CI1" t="s">
         <v>84</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CJ1" t="s">
         <v>85</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="CK1" t="s">
+        <v>147</v>
+      </c>
+      <c r="CL1" t="s">
         <v>86</v>
       </c>
-      <c r="CK1" t="s">
-        <v>148</v>
-      </c>
-      <c r="CL1" t="s">
+      <c r="CM1" t="s">
         <v>87</v>
       </c>
-      <c r="CM1" t="s">
+      <c r="CN1" t="s">
         <v>88</v>
       </c>
-      <c r="CN1" t="s">
+      <c r="CO1" t="s">
         <v>89</v>
       </c>
-      <c r="CO1" t="s">
+      <c r="CP1" t="s">
         <v>90</v>
       </c>
-      <c r="CP1" t="s">
+      <c r="CQ1" t="s">
         <v>91</v>
       </c>
-      <c r="CQ1" t="s">
+      <c r="CR1" t="s">
         <v>92</v>
       </c>
-      <c r="CR1" t="s">
+      <c r="CS1" t="s">
         <v>93</v>
       </c>
-      <c r="CS1" t="s">
+      <c r="CT1" t="s">
         <v>94</v>
       </c>
-      <c r="CT1" t="s">
+      <c r="CU1" t="s">
         <v>95</v>
       </c>
-      <c r="CU1" t="s">
+      <c r="CV1" t="s">
         <v>96</v>
       </c>
-      <c r="CV1" t="s">
+      <c r="CW1" t="s">
         <v>97</v>
       </c>
-      <c r="CW1" t="s">
+      <c r="CX1" t="s">
         <v>98</v>
       </c>
-      <c r="CX1" t="s">
+      <c r="CY1" t="s">
         <v>99</v>
       </c>
-      <c r="CY1" t="s">
+      <c r="CZ1" t="s">
         <v>100</v>
       </c>
-      <c r="CZ1" t="s">
+      <c r="DA1" t="s">
         <v>101</v>
       </c>
-      <c r="DA1" t="s">
+      <c r="DB1" t="s">
         <v>102</v>
       </c>
-      <c r="DB1" t="s">
+      <c r="DC1" t="s">
         <v>103</v>
       </c>
-      <c r="DC1" t="s">
+      <c r="DD1" t="s">
         <v>104</v>
       </c>
-      <c r="DD1" t="s">
+      <c r="DE1" t="s">
         <v>105</v>
       </c>
-      <c r="DE1" t="s">
+      <c r="DF1" t="s">
         <v>106</v>
       </c>
-      <c r="DF1" t="s">
+      <c r="DG1" t="s">
         <v>107</v>
       </c>
-      <c r="DG1" t="s">
+      <c r="DH1" t="s">
         <v>108</v>
       </c>
-      <c r="DH1" t="s">
+      <c r="DI1" t="s">
         <v>109</v>
       </c>
-      <c r="DI1" t="s">
+      <c r="DJ1" t="s">
         <v>110</v>
       </c>
-      <c r="DJ1" t="s">
+      <c r="DK1" t="s">
         <v>111</v>
       </c>
-      <c r="DK1" t="s">
+      <c r="DL1" t="s">
         <v>112</v>
       </c>
-      <c r="DL1" t="s">
+      <c r="DM1" t="s">
         <v>113</v>
       </c>
-      <c r="DM1" t="s">
+      <c r="DN1" t="s">
         <v>114</v>
       </c>
-      <c r="DN1" t="s">
+      <c r="DO1" t="s">
         <v>115</v>
       </c>
-      <c r="DO1" t="s">
+      <c r="DP1" t="s">
         <v>116</v>
       </c>
-      <c r="DP1" t="s">
+      <c r="DQ1" t="s">
         <v>117</v>
       </c>
-      <c r="DQ1" t="s">
+      <c r="DR1" t="s">
         <v>118</v>
       </c>
-      <c r="DR1" t="s">
+      <c r="DS1" t="s">
         <v>119</v>
       </c>
-      <c r="DS1" t="s">
+      <c r="DT1" t="s">
         <v>120</v>
       </c>
-      <c r="DT1" t="s">
+      <c r="DU1" t="s">
         <v>121</v>
       </c>
-      <c r="DU1" t="s">
+      <c r="DV1" t="s">
         <v>122</v>
       </c>
-      <c r="DV1" t="s">
+      <c r="DW1" t="s">
         <v>123</v>
       </c>
-      <c r="DW1" t="s">
+      <c r="DX1" t="s">
         <v>124</v>
       </c>
-      <c r="DX1" t="s">
+      <c r="DY1" t="s">
         <v>125</v>
       </c>
-      <c r="DY1" t="s">
+      <c r="DZ1" t="s">
         <v>126</v>
       </c>
-      <c r="DZ1" t="s">
+      <c r="EA1" t="s">
         <v>127</v>
       </c>
-      <c r="EA1" t="s">
+      <c r="EB1" t="s">
         <v>128</v>
       </c>
-      <c r="EB1" t="s">
+      <c r="EC1" t="s">
         <v>129</v>
       </c>
-      <c r="EC1" t="s">
+      <c r="ED1" t="s">
         <v>130</v>
       </c>
-      <c r="ED1" t="s">
+      <c r="EE1" t="s">
         <v>131</v>
       </c>
-      <c r="EE1" t="s">
+      <c r="EF1" t="s">
         <v>132</v>
       </c>
-      <c r="EF1" t="s">
+      <c r="EG1" t="s">
         <v>133</v>
       </c>
-      <c r="EG1" t="s">
+      <c r="EH1" t="s">
         <v>134</v>
       </c>
-      <c r="EH1" t="s">
+      <c r="EI1" t="s">
         <v>135</v>
       </c>
-      <c r="EI1" t="s">
+      <c r="EJ1" t="s">
         <v>136</v>
       </c>
-      <c r="EJ1" t="s">
+      <c r="EK1" t="s">
         <v>137</v>
       </c>
-      <c r="EK1" t="s">
+      <c r="EL1" t="s">
         <v>138</v>
       </c>
-      <c r="EL1" t="s">
+      <c r="EM1" t="s">
         <v>139</v>
       </c>
-      <c r="EM1" t="s">
+      <c r="EN1" t="s">
         <v>140</v>
       </c>
-      <c r="EN1" t="s">
+      <c r="EO1" t="s">
         <v>141</v>
       </c>
-      <c r="EO1" t="s">
+      <c r="EP1" t="s">
         <v>142</v>
       </c>
-      <c r="EP1" t="s">
+      <c r="EQ1" t="s">
         <v>143</v>
       </c>
-      <c r="EQ1" t="s">
+      <c r="ER1" t="s">
         <v>144</v>
       </c>
-      <c r="ER1" t="s">
+      <c r="ES1" t="s">
         <v>145</v>
       </c>
-      <c r="ES1" t="s">
+      <c r="ET1" t="s">
         <v>146</v>
-      </c>
-      <c r="ET1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="2" spans="2:150" x14ac:dyDescent="0.3">
@@ -1293,50 +1307,50 @@
       <c r="C2">
         <v>50</v>
       </c>
-      <c r="D2">
-        <v>270</v>
+      <c r="D2" s="1">
+        <v>200</v>
       </c>
       <c r="E2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>2400</v>
+        <v>148</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2000</v>
       </c>
       <c r="G2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="H2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="I2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="J2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="K2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="L2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="M2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="O2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="P2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="Q2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="R2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="S2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="T2">
         <v>36.4</v>
@@ -1365,7 +1379,7 @@
       <c r="AB2">
         <v>0.9</v>
       </c>
-      <c r="AC2">
+      <c r="AC2" s="1">
         <v>4000</v>
       </c>
       <c r="AD2">
@@ -1375,64 +1389,64 @@
         <v>55</v>
       </c>
       <c r="AF2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AG2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AH2">
         <v>625</v>
       </c>
       <c r="AI2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AJ2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AK2">
         <v>15</v>
       </c>
       <c r="AL2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AM2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AN2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AO2">
         <v>5</v>
       </c>
       <c r="AP2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AQ2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AR2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AS2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AT2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AU2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AV2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AW2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AX2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AY2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AZ2">
         <v>90</v>
@@ -1455,32 +1469,32 @@
       <c r="BF2">
         <v>400</v>
       </c>
-      <c r="BG2" t="s">
-        <v>0</v>
+      <c r="BG2">
+        <v>2</v>
       </c>
       <c r="BH2">
         <v>550</v>
       </c>
       <c r="BI2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="BJ2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="BK2">
         <v>100</v>
       </c>
       <c r="BL2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="BM2">
         <v>400</v>
       </c>
       <c r="BN2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="BO2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="BP2">
         <v>0.35000000000000003</v>
@@ -1513,282 +1527,282 @@
         <v>1.4000000000000001</v>
       </c>
       <c r="BZ2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CA2">
         <v>0.98</v>
       </c>
       <c r="CB2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CC2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CD2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CE2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CF2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CG2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CH2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CI2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CJ2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CK2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CL2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CM2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CN2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CO2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CP2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CQ2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CR2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CS2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CT2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CU2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CV2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CW2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CX2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CY2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CZ2" t="s">
-        <v>0</v>
-      </c>
-      <c r="DA2">
+        <v>148</v>
+      </c>
+      <c r="DA2" s="1">
         <v>0.25</v>
       </c>
       <c r="DB2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DC2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DD2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DE2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DF2" t="s">
-        <v>0</v>
-      </c>
-      <c r="DG2">
+        <v>148</v>
+      </c>
+      <c r="DG2" s="1">
         <v>0.25</v>
       </c>
       <c r="DH2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DI2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DJ2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DK2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DL2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DM2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DN2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DO2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DP2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DQ2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DR2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DS2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DT2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DU2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DV2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DW2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DX2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DY2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DZ2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="EA2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="EB2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="EC2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="ED2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="EE2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="EF2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="EG2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="EH2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="EI2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="EJ2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="EK2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="EL2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="EM2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="EN2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="EO2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="EP2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="EQ2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="ER2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="ES2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="ET2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="2:150" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>94</v>
+        <v>148</v>
+      </c>
+      <c r="C3" s="1">
+        <v>85</v>
       </c>
       <c r="D3">
         <v>422.5</v>
       </c>
       <c r="E3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="F3">
         <v>2600</v>
       </c>
       <c r="G3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="H3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="I3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="J3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="K3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="L3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="M3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="N3">
         <v>2700</v>
       </c>
       <c r="O3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="P3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="Q3" t="s">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>60</v>
+        <v>148</v>
+      </c>
+      <c r="R3" s="2">
+        <v>50</v>
       </c>
       <c r="S3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="T3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="U3">
         <v>2500</v>
@@ -1803,7 +1817,7 @@
         <v>4000</v>
       </c>
       <c r="Y3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="Z3">
         <v>2300</v>
@@ -1814,7 +1828,7 @@
       <c r="AB3">
         <v>10</v>
       </c>
-      <c r="AC3">
+      <c r="AC3" s="1">
         <v>10000</v>
       </c>
       <c r="AD3">
@@ -1824,79 +1838,79 @@
         <v>400</v>
       </c>
       <c r="AF3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AG3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AH3">
         <v>3000</v>
       </c>
       <c r="AI3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AJ3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AK3">
         <v>1000</v>
       </c>
       <c r="AL3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AM3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AN3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AO3">
         <v>50</v>
       </c>
       <c r="AP3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AQ3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AR3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AS3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AT3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AU3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AV3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AW3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AX3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AY3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AZ3">
         <v>2000</v>
       </c>
       <c r="BA3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="BB3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="BC3">
         <v>35</v>
       </c>
       <c r="BD3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="BE3">
         <v>100</v>
@@ -1904,95 +1918,92 @@
       <c r="BF3">
         <v>1000</v>
       </c>
-      <c r="BG3">
-        <v>2</v>
-      </c>
       <c r="BH3">
         <v>3500</v>
       </c>
       <c r="BI3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="BJ3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="BK3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="BL3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="BM3">
         <v>1000</v>
       </c>
       <c r="BN3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="BO3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="BP3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="BQ3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="BR3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="BS3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="BT3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="BU3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="BV3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="BW3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="BX3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="BY3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="BZ3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CA3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CB3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CC3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CD3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CE3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CF3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CG3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CH3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CI3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CJ3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CK3">
         <v>200</v>
@@ -2004,181 +2015,181 @@
         <v>28.8</v>
       </c>
       <c r="CN3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CO3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CP3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CQ3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CR3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CS3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CT3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CU3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CV3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CW3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CX3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CY3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="CZ3" t="s">
-        <v>0</v>
-      </c>
-      <c r="DA3" t="s">
-        <v>0</v>
+        <v>148</v>
+      </c>
+      <c r="DA3" s="1" t="s">
+        <v>148</v>
       </c>
       <c r="DB3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DC3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DD3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DE3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DF3" t="s">
-        <v>0</v>
-      </c>
-      <c r="DG3" t="s">
-        <v>0</v>
+        <v>148</v>
+      </c>
+      <c r="DG3" s="1" t="s">
+        <v>148</v>
       </c>
       <c r="DH3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DI3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DJ3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DK3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DL3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DM3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DN3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DO3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DP3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DQ3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DR3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DS3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DT3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DU3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DV3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DW3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DX3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DY3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="DZ3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="EA3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="EB3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="EC3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="ED3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="EE3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="EF3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="EG3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="EH3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="EI3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="EJ3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="EK3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="EL3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="EM3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="EN3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="EO3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="EP3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="EQ3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="ER3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="ES3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="ET3" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="2:150" x14ac:dyDescent="0.3">
@@ -2263,8 +2274,8 @@
       <c r="AB4">
         <v>1</v>
       </c>
-      <c r="AC4">
-        <v>1</v>
+      <c r="AC4" s="1">
+        <v>0</v>
       </c>
       <c r="AD4">
         <v>1</v>
@@ -2492,7 +2503,7 @@
         <v>0</v>
       </c>
       <c r="DA4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DB4">
         <v>0</v>
@@ -2510,7 +2521,7 @@
         <v>0</v>
       </c>
       <c r="DG4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DH4">
         <v>0</v>
@@ -2631,6 +2642,56 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B5:KMT5 EU2:KMT4">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="EU2:KMT2">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="EU3:KMT3">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="EU4:KMT4">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:KMT5">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B4:ET4">
     <cfRule type="colorScale" priority="1">
       <colorScale>

</xml_diff>